<commit_message>
General update & clean up
</commit_message>
<xml_diff>
--- a/Datasets/Biomarker_discovery/Biomarkers_Nerea_predictions.xlsx
+++ b/Datasets/Biomarker_discovery/Biomarkers_Nerea_predictions.xlsx
@@ -25,10 +25,10 @@
     <t>Protein name</t>
   </si>
   <si>
-    <t>CSF_proba</t>
-  </si>
-  <si>
-    <t>CSF_proba_3plus</t>
+    <t>lr_l2</t>
+  </si>
+  <si>
+    <t>lr_l2_3plus</t>
   </si>
   <si>
     <t>Q9Y6Q6</t>
@@ -2646,10 +2646,10 @@
         <v>584</v>
       </c>
       <c r="D2">
-        <v>0.8784438731900869</v>
+        <v>0.8797564139965099</v>
       </c>
       <c r="E2">
-        <v>0.92562406631143</v>
+        <v>0.8571374600644135</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -2663,10 +2663,10 @@
         <v>585</v>
       </c>
       <c r="D3">
-        <v>0.4345001973541399</v>
+        <v>0.4480448477293726</v>
       </c>
       <c r="E3">
-        <v>0.2683718668771786</v>
+        <v>0.3809094178080927</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -2680,10 +2680,10 @@
         <v>586</v>
       </c>
       <c r="D4">
-        <v>0.9020962501162245</v>
+        <v>0.9222244094138071</v>
       </c>
       <c r="E4">
-        <v>0.9688078143078116</v>
+        <v>0.9562995438583957</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -2697,10 +2697,10 @@
         <v>587</v>
       </c>
       <c r="D5">
-        <v>0.7905707829693092</v>
+        <v>0.8298598614815995</v>
       </c>
       <c r="E5">
-        <v>0.9539068839387824</v>
+        <v>0.8978535528154969</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -2714,10 +2714,10 @@
         <v>588</v>
       </c>
       <c r="D6">
-        <v>0.4177778828002421</v>
+        <v>0.3835548344538336</v>
       </c>
       <c r="E6">
-        <v>0.1427177621479126</v>
+        <v>0.1834051990390966</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -2731,10 +2731,10 @@
         <v>300</v>
       </c>
       <c r="D7">
-        <v>0.6466319356164462</v>
+        <v>0.5505007820938242</v>
       </c>
       <c r="E7">
-        <v>0.7330822358889777</v>
+        <v>0.5986327078970334</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -2748,10 +2748,10 @@
         <v>301</v>
       </c>
       <c r="D8">
-        <v>0.8707141752430329</v>
+        <v>0.9045372484294808</v>
       </c>
       <c r="E8">
-        <v>0.9725323199111986</v>
+        <v>0.9709281927374021</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -2765,10 +2765,10 @@
         <v>589</v>
       </c>
       <c r="D9">
-        <v>0.6985299235042741</v>
+        <v>0.6408076786148044</v>
       </c>
       <c r="E9">
-        <v>0.8392698675048043</v>
+        <v>0.7866470878924857</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -2782,10 +2782,10 @@
         <v>303</v>
       </c>
       <c r="D10">
-        <v>0.5804721889224199</v>
+        <v>0.6930539832486046</v>
       </c>
       <c r="E10">
-        <v>0.5723741916779317</v>
+        <v>0.8156176114185262</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -2799,10 +2799,10 @@
         <v>590</v>
       </c>
       <c r="D11">
-        <v>0.4090097931083643</v>
+        <v>0.3137652887464821</v>
       </c>
       <c r="E11">
-        <v>0.214858375391756</v>
+        <v>0.1809866018896065</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -2816,10 +2816,10 @@
         <v>305</v>
       </c>
       <c r="D12">
-        <v>0.6514329664608814</v>
+        <v>0.6400344957306753</v>
       </c>
       <c r="E12">
-        <v>0.8014301326700204</v>
+        <v>0.7136251531697805</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -2832,12 +2832,6 @@
       <c r="C13" t="s">
         <v>306</v>
       </c>
-      <c r="D13">
-        <v>0.2867358642429288</v>
-      </c>
-      <c r="E13">
-        <v>0.2296551429884344</v>
-      </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
@@ -2850,10 +2844,10 @@
         <v>591</v>
       </c>
       <c r="D14">
-        <v>0.6585596004887332</v>
+        <v>0.5946019483675351</v>
       </c>
       <c r="E14">
-        <v>0.4046835876243963</v>
+        <v>0.3566840374619789</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -2867,10 +2861,10 @@
         <v>592</v>
       </c>
       <c r="D15">
-        <v>0.8802947840315861</v>
+        <v>0.8949480996514343</v>
       </c>
       <c r="E15">
-        <v>0.9450477797154841</v>
+        <v>0.945225211752016</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -2884,10 +2878,10 @@
         <v>593</v>
       </c>
       <c r="D16">
-        <v>0.8375571550824235</v>
+        <v>0.9223323720746543</v>
       </c>
       <c r="E16">
-        <v>0.8819733420074307</v>
+        <v>0.9065934663661653</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -2901,10 +2895,10 @@
         <v>310</v>
       </c>
       <c r="D17">
-        <v>0.4463051520006088</v>
+        <v>0.4768165843176602</v>
       </c>
       <c r="E17">
-        <v>0.2179793447077973</v>
+        <v>0.2035644197923049</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -2918,10 +2912,10 @@
         <v>594</v>
       </c>
       <c r="D18">
-        <v>0.1534714642558646</v>
+        <v>0.1816407328212107</v>
       </c>
       <c r="E18">
-        <v>0.03179808979800768</v>
+        <v>0.07740149629459379</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -2935,10 +2929,10 @@
         <v>312</v>
       </c>
       <c r="D19">
-        <v>0.8591241423702204</v>
+        <v>0.8927950161760109</v>
       </c>
       <c r="E19">
-        <v>0.9119426116262731</v>
+        <v>0.9613237356867481</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -2952,10 +2946,10 @@
         <v>313</v>
       </c>
       <c r="D20">
-        <v>0.9313455567660475</v>
+        <v>0.9332938020315883</v>
       </c>
       <c r="E20">
-        <v>0.9750456109154125</v>
+        <v>0.9823654118905691</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -2969,10 +2963,10 @@
         <v>595</v>
       </c>
       <c r="D21">
-        <v>0.2542521034278826</v>
+        <v>0.2980571588087156</v>
       </c>
       <c r="E21">
-        <v>0.41267769006052</v>
+        <v>0.4163984915943915</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -2986,10 +2980,10 @@
         <v>315</v>
       </c>
       <c r="D22">
-        <v>0.6484113699361341</v>
+        <v>0.5468910204387565</v>
       </c>
       <c r="E22">
-        <v>0.5246045551252299</v>
+        <v>0.3868720428464156</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -3003,10 +2997,10 @@
         <v>316</v>
       </c>
       <c r="D23">
-        <v>0.919944442471889</v>
+        <v>0.866562963896147</v>
       </c>
       <c r="E23">
-        <v>0.9399341524127245</v>
+        <v>0.8782079038151832</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -3020,10 +3014,10 @@
         <v>596</v>
       </c>
       <c r="D24">
-        <v>0.756720547740669</v>
+        <v>0.7474117217302931</v>
       </c>
       <c r="E24">
-        <v>0.7318248635608461</v>
+        <v>0.7511985539110111</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -3037,10 +3031,10 @@
         <v>597</v>
       </c>
       <c r="D25">
-        <v>0.8830378045406448</v>
+        <v>0.9248580597368956</v>
       </c>
       <c r="E25">
-        <v>0.973079656986376</v>
+        <v>0.9684548084013831</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -3054,10 +3048,10 @@
         <v>598</v>
       </c>
       <c r="D26">
-        <v>0.8573115081858108</v>
+        <v>0.8704638215275335</v>
       </c>
       <c r="E26">
-        <v>0.9078522068647683</v>
+        <v>0.9111659090724122</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -3071,10 +3065,10 @@
         <v>599</v>
       </c>
       <c r="D27">
-        <v>0.8426702623594626</v>
+        <v>0.7454937524859399</v>
       </c>
       <c r="E27">
-        <v>0.9198282582208741</v>
+        <v>0.841611246262981</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -3088,10 +3082,10 @@
         <v>321</v>
       </c>
       <c r="D28">
-        <v>0.7628222106670706</v>
+        <v>0.8250862075099188</v>
       </c>
       <c r="E28">
-        <v>0.6504567029193675</v>
+        <v>0.8115031066330048</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -3105,10 +3099,10 @@
         <v>600</v>
       </c>
       <c r="D29">
-        <v>0.7792381430354108</v>
+        <v>0.8453811045503473</v>
       </c>
       <c r="E29">
-        <v>0.9202018518828322</v>
+        <v>0.9330437968127142</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -3122,10 +3116,10 @@
         <v>323</v>
       </c>
       <c r="D30">
-        <v>0.491876690342299</v>
+        <v>0.4691797198446181</v>
       </c>
       <c r="E30">
-        <v>0.5860113346232724</v>
+        <v>0.6580611691593445</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -3139,10 +3133,10 @@
         <v>324</v>
       </c>
       <c r="D31">
-        <v>0.7955713270958611</v>
+        <v>0.810996425388097</v>
       </c>
       <c r="E31">
-        <v>0.8928578255692312</v>
+        <v>0.8866038055745217</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -3156,10 +3150,10 @@
         <v>601</v>
       </c>
       <c r="D32">
-        <v>0.814095934315626</v>
+        <v>0.779155979016623</v>
       </c>
       <c r="E32">
-        <v>0.9430262734709975</v>
+        <v>0.8700964220558669</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -3173,10 +3167,10 @@
         <v>602</v>
       </c>
       <c r="D33">
-        <v>0.2499601874252655</v>
+        <v>0.1691087061300373</v>
       </c>
       <c r="E33">
-        <v>0.1804296331004656</v>
+        <v>0.3119439598093434</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -3190,10 +3184,10 @@
         <v>603</v>
       </c>
       <c r="D34">
-        <v>0.3280090827604166</v>
+        <v>0.3499001784968603</v>
       </c>
       <c r="E34">
-        <v>0.1256257370380488</v>
+        <v>0.206542800403806</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -3207,10 +3201,10 @@
         <v>604</v>
       </c>
       <c r="D35">
-        <v>0.8129937537983454</v>
+        <v>0.8108759551839052</v>
       </c>
       <c r="E35">
-        <v>0.9554222548955068</v>
+        <v>0.8824617675227878</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -3224,10 +3218,10 @@
         <v>329</v>
       </c>
       <c r="D36">
-        <v>0.8146141524307029</v>
+        <v>0.7816894742973989</v>
       </c>
       <c r="E36">
-        <v>0.8540919332038449</v>
+        <v>0.821270630034562</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -3241,10 +3235,10 @@
         <v>605</v>
       </c>
       <c r="D37">
-        <v>0.860437820535908</v>
+        <v>0.9172730372520422</v>
       </c>
       <c r="E37">
-        <v>0.8422297010976909</v>
+        <v>0.8919723732237131</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -3258,10 +3252,10 @@
         <v>331</v>
       </c>
       <c r="D38">
-        <v>0.8018089755252031</v>
+        <v>0.8042573779068791</v>
       </c>
       <c r="E38">
-        <v>0.9082058114968043</v>
+        <v>0.9098931320081095</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -3275,10 +3269,10 @@
         <v>332</v>
       </c>
       <c r="D39">
-        <v>0.8556390134493435</v>
+        <v>0.8164685308867288</v>
       </c>
       <c r="E39">
-        <v>0.9399313473287052</v>
+        <v>0.8707165188794835</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -3292,10 +3286,10 @@
         <v>606</v>
       </c>
       <c r="D40">
-        <v>0.8977378407160632</v>
+        <v>0.8924088580977693</v>
       </c>
       <c r="E40">
-        <v>0.9895257975126165</v>
+        <v>0.9171722006221178</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -3309,10 +3303,10 @@
         <v>607</v>
       </c>
       <c r="D41">
-        <v>0.2871758404876708</v>
+        <v>0.2969954360375174</v>
       </c>
       <c r="E41">
-        <v>0.1171380254545851</v>
+        <v>0.1748727898656194</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -3326,10 +3320,10 @@
         <v>608</v>
       </c>
       <c r="D42">
-        <v>0.6857513021350236</v>
+        <v>0.7098148014785252</v>
       </c>
       <c r="E42">
-        <v>0.5568732121958847</v>
+        <v>0.6949071679390083</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -3343,10 +3337,10 @@
         <v>609</v>
       </c>
       <c r="D43">
-        <v>0.7333005532718071</v>
+        <v>0.7873115340663693</v>
       </c>
       <c r="E43">
-        <v>0.9147198529596502</v>
+        <v>0.9314922902254235</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -3360,10 +3354,10 @@
         <v>337</v>
       </c>
       <c r="D44">
-        <v>0.4184077981760354</v>
+        <v>0.4477242587764854</v>
       </c>
       <c r="E44">
-        <v>0.2507248359946127</v>
+        <v>0.2047247059551583</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -3377,10 +3371,10 @@
         <v>610</v>
       </c>
       <c r="D45">
-        <v>0.9478461892324218</v>
+        <v>0.9099908345073632</v>
       </c>
       <c r="E45">
-        <v>0.9724346000509557</v>
+        <v>0.9645373507765822</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -3394,10 +3388,10 @@
         <v>339</v>
       </c>
       <c r="D46">
-        <v>0.8537244451707561</v>
+        <v>0.8999933215553713</v>
       </c>
       <c r="E46">
-        <v>0.9365161187209885</v>
+        <v>0.9413128737440214</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -3411,10 +3405,10 @@
         <v>611</v>
       </c>
       <c r="D47">
-        <v>0.7267005494026865</v>
+        <v>0.6702053109767692</v>
       </c>
       <c r="E47">
-        <v>0.7177619038165064</v>
+        <v>0.7525407468743922</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -3428,10 +3422,10 @@
         <v>612</v>
       </c>
       <c r="D48">
-        <v>0.7246958367692649</v>
+        <v>0.7576124060612562</v>
       </c>
       <c r="E48">
-        <v>0.8147288919612041</v>
+        <v>0.8206180948259263</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -3445,10 +3439,10 @@
         <v>613</v>
       </c>
       <c r="D49">
-        <v>0.7690153832017048</v>
+        <v>0.6623453834725648</v>
       </c>
       <c r="E49">
-        <v>0.9006796214094173</v>
+        <v>0.5832725960018434</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -3462,10 +3456,10 @@
         <v>343</v>
       </c>
       <c r="D50">
-        <v>0.8568970510788493</v>
+        <v>0.8002693274096208</v>
       </c>
       <c r="E50">
-        <v>0.8907232481453097</v>
+        <v>0.8772414727184364</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -3479,10 +3473,10 @@
         <v>344</v>
       </c>
       <c r="D51">
-        <v>0.8032721934285114</v>
+        <v>0.7590161849022862</v>
       </c>
       <c r="E51">
-        <v>0.8668410804636708</v>
+        <v>0.8431315667963871</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -3496,10 +3490,10 @@
         <v>345</v>
       </c>
       <c r="D52">
-        <v>0.9901040321143704</v>
+        <v>0.9708427179507338</v>
       </c>
       <c r="E52">
-        <v>0.9940949462672446</v>
+        <v>0.9959643090581012</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -3513,10 +3507,10 @@
         <v>614</v>
       </c>
       <c r="D53">
-        <v>0.9787594862869579</v>
+        <v>0.9707154962532221</v>
       </c>
       <c r="E53">
-        <v>0.9973132200398286</v>
+        <v>0.9705113735632382</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -3530,10 +3524,10 @@
         <v>615</v>
       </c>
       <c r="D54">
-        <v>0.8577574156621408</v>
+        <v>0.8730553229483825</v>
       </c>
       <c r="E54">
-        <v>0.9733504115532784</v>
+        <v>0.9310547966732909</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -3547,10 +3541,10 @@
         <v>348</v>
       </c>
       <c r="D55">
-        <v>0.3704478241123073</v>
+        <v>0.3180753092075642</v>
       </c>
       <c r="E55">
-        <v>0.7562709794434289</v>
+        <v>0.5564270005824118</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -3564,10 +3558,10 @@
         <v>349</v>
       </c>
       <c r="D56">
-        <v>0.4476565829861804</v>
+        <v>0.4500188935314302</v>
       </c>
       <c r="E56">
-        <v>0.1794292776365657</v>
+        <v>0.1889812810481979</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -3581,10 +3575,10 @@
         <v>616</v>
       </c>
       <c r="D57">
-        <v>0.262605965684695</v>
+        <v>0.2149080616630376</v>
       </c>
       <c r="E57">
-        <v>0.09117977954445708</v>
+        <v>0.08783867528183516</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -3598,10 +3592,10 @@
         <v>617</v>
       </c>
       <c r="D58">
-        <v>0.5585032991821604</v>
+        <v>0.7217357818193334</v>
       </c>
       <c r="E58">
-        <v>0.388539831400796</v>
+        <v>0.5628131899880132</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -3615,10 +3609,10 @@
         <v>352</v>
       </c>
       <c r="D59">
-        <v>0.4560102158154599</v>
+        <v>0.2623552004706742</v>
       </c>
       <c r="E59">
-        <v>0.3601130106000613</v>
+        <v>0.1918496198216256</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -3632,10 +3626,10 @@
         <v>353</v>
       </c>
       <c r="D60">
-        <v>0.8970062088487917</v>
+        <v>0.8792027620062564</v>
       </c>
       <c r="E60">
-        <v>0.970794757708013</v>
+        <v>0.9515054605579797</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -3649,10 +3643,10 @@
         <v>354</v>
       </c>
       <c r="D61">
-        <v>0.6947044188090342</v>
+        <v>0.6659950571307385</v>
       </c>
       <c r="E61">
-        <v>0.8469930139029552</v>
+        <v>0.7483309406803722</v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -3666,10 +3660,10 @@
         <v>618</v>
       </c>
       <c r="D62">
-        <v>0.4032676256332632</v>
+        <v>0.3894594894946061</v>
       </c>
       <c r="E62">
-        <v>0.2743595904366474</v>
+        <v>0.177465101958823</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -3683,10 +3677,10 @@
         <v>619</v>
       </c>
       <c r="D63">
-        <v>0.819459432167154</v>
+        <v>0.8677388855580103</v>
       </c>
       <c r="E63">
-        <v>0.925552149545923</v>
+        <v>0.8859128597441692</v>
       </c>
     </row>
     <row r="64" spans="1:5">
@@ -3700,10 +3694,10 @@
         <v>357</v>
       </c>
       <c r="D64">
-        <v>0.3475696558198352</v>
+        <v>0.4929618291926627</v>
       </c>
       <c r="E64">
-        <v>0.2081488052573895</v>
+        <v>0.6318990558927369</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -3717,10 +3711,10 @@
         <v>620</v>
       </c>
       <c r="D65">
-        <v>0.6670544828312883</v>
+        <v>0.6446605430655555</v>
       </c>
       <c r="E65">
-        <v>0.4749524806027847</v>
+        <v>0.658376655850115</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -3734,10 +3728,10 @@
         <v>621</v>
       </c>
       <c r="D66">
-        <v>0.790914630519354</v>
+        <v>0.7878785470521947</v>
       </c>
       <c r="E66">
-        <v>0.9335112360145587</v>
+        <v>0.7759551533489351</v>
       </c>
     </row>
     <row r="67" spans="1:5">
@@ -3751,10 +3745,10 @@
         <v>622</v>
       </c>
       <c r="D67">
-        <v>0.4294651965309257</v>
+        <v>0.2994434302309838</v>
       </c>
       <c r="E67">
-        <v>0.2242610078972323</v>
+        <v>0.4542997151698788</v>
       </c>
     </row>
     <row r="68" spans="1:5">
@@ -3768,10 +3762,10 @@
         <v>623</v>
       </c>
       <c r="D68">
-        <v>0.9733548102849134</v>
+        <v>0.9755216418752248</v>
       </c>
       <c r="E68">
-        <v>0.9915462707524877</v>
+        <v>0.9969105954925536</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -3785,10 +3779,10 @@
         <v>362</v>
       </c>
       <c r="D69">
-        <v>0.4286789135710692</v>
+        <v>0.368885859732386</v>
       </c>
       <c r="E69">
-        <v>0.1839426544030301</v>
+        <v>0.5062217848116389</v>
       </c>
     </row>
     <row r="70" spans="1:5">
@@ -3802,10 +3796,10 @@
         <v>624</v>
       </c>
       <c r="D70">
-        <v>0.5570246799034466</v>
+        <v>0.6944656893828735</v>
       </c>
       <c r="E70">
-        <v>0.4938668855899511</v>
+        <v>0.4228172377644507</v>
       </c>
     </row>
     <row r="71" spans="1:5">
@@ -3819,10 +3813,10 @@
         <v>364</v>
       </c>
       <c r="D71">
-        <v>0.8033179699882117</v>
+        <v>0.8473734854641407</v>
       </c>
       <c r="E71">
-        <v>0.570525861417295</v>
+        <v>0.8892047276061754</v>
       </c>
     </row>
     <row r="72" spans="1:5">
@@ -3836,10 +3830,10 @@
         <v>365</v>
       </c>
       <c r="D72">
-        <v>0.3339349577281063</v>
+        <v>0.4890955891584443</v>
       </c>
       <c r="E72">
-        <v>0.4111046511827436</v>
+        <v>0.6846524602137676</v>
       </c>
     </row>
     <row r="73" spans="1:5">
@@ -3853,10 +3847,10 @@
         <v>366</v>
       </c>
       <c r="D73">
-        <v>0.9042864039142412</v>
+        <v>0.8837474016134058</v>
       </c>
       <c r="E73">
-        <v>0.9404764084476477</v>
+        <v>0.9444478470102535</v>
       </c>
     </row>
     <row r="74" spans="1:5">
@@ -3870,10 +3864,10 @@
         <v>367</v>
       </c>
       <c r="D74">
-        <v>0.6914924095991442</v>
+        <v>0.5539438062064858</v>
       </c>
       <c r="E74">
-        <v>0.6833172743685846</v>
+        <v>0.8117048866639117</v>
       </c>
     </row>
     <row r="75" spans="1:5">
@@ -3887,10 +3881,10 @@
         <v>625</v>
       </c>
       <c r="D75">
-        <v>0.7881391283935428</v>
+        <v>0.7894639544379112</v>
       </c>
       <c r="E75">
-        <v>0.9008624263499494</v>
+        <v>0.8568974424751505</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -3904,10 +3898,10 @@
         <v>626</v>
       </c>
       <c r="D76">
-        <v>0.7722898364443238</v>
+        <v>0.8035594168878493</v>
       </c>
       <c r="E76">
-        <v>0.7323923501213216</v>
+        <v>0.8276829359768689</v>
       </c>
     </row>
     <row r="77" spans="1:5">
@@ -3921,10 +3915,10 @@
         <v>627</v>
       </c>
       <c r="D77">
-        <v>0.9875031936030155</v>
+        <v>0.9685858449077012</v>
       </c>
       <c r="E77">
-        <v>0.9975153184558186</v>
+        <v>0.9970525292311824</v>
       </c>
     </row>
     <row r="78" spans="1:5">
@@ -3938,10 +3932,10 @@
         <v>628</v>
       </c>
       <c r="D78">
-        <v>0.6402603160818445</v>
+        <v>0.7686834388825959</v>
       </c>
       <c r="E78">
-        <v>0.6914998811837696</v>
+        <v>0.6751952457051515</v>
       </c>
     </row>
     <row r="79" spans="1:5">
@@ -3955,10 +3949,10 @@
         <v>629</v>
       </c>
       <c r="D79">
-        <v>0.4513335398851838</v>
+        <v>0.3910507726131077</v>
       </c>
       <c r="E79">
-        <v>0.3432870044071477</v>
+        <v>0.3157966783098296</v>
       </c>
     </row>
     <row r="80" spans="1:5">
@@ -3972,10 +3966,10 @@
         <v>630</v>
       </c>
       <c r="D80">
-        <v>0.9500874822781319</v>
+        <v>0.9276744078099257</v>
       </c>
       <c r="E80">
-        <v>0.9859629061311004</v>
+        <v>0.9753419242650738</v>
       </c>
     </row>
     <row r="81" spans="1:5">
@@ -3986,10 +3980,10 @@
         <v>631</v>
       </c>
       <c r="D81">
-        <v>0.9427701458944212</v>
+        <v>0.9813727213071058</v>
       </c>
       <c r="E81">
-        <v>0.9537759614085962</v>
+        <v>0.9800691047298241</v>
       </c>
     </row>
     <row r="82" spans="1:5">
@@ -4003,10 +3997,10 @@
         <v>374</v>
       </c>
       <c r="D82">
-        <v>0.4055614071151944</v>
+        <v>0.2794750712412616</v>
       </c>
       <c r="E82">
-        <v>0.1302007242193888</v>
+        <v>0.1653644452105625</v>
       </c>
     </row>
     <row r="83" spans="1:5">
@@ -4020,10 +4014,10 @@
         <v>375</v>
       </c>
       <c r="D83">
-        <v>0.6744294710428373</v>
+        <v>0.5165931739059713</v>
       </c>
       <c r="E83">
-        <v>0.7353954631037484</v>
+        <v>0.8421124487016663</v>
       </c>
     </row>
     <row r="84" spans="1:5">
@@ -4037,10 +4031,10 @@
         <v>376</v>
       </c>
       <c r="D84">
-        <v>0.53725554683849</v>
+        <v>0.7115185472422269</v>
       </c>
       <c r="E84">
-        <v>0.5345636097937869</v>
+        <v>0.4917993484089849</v>
       </c>
     </row>
     <row r="85" spans="1:5">
@@ -4054,10 +4048,10 @@
         <v>377</v>
       </c>
       <c r="D85">
-        <v>0.3064117411876804</v>
+        <v>0.3370869185555706</v>
       </c>
       <c r="E85">
-        <v>0.1910294753575625</v>
+        <v>0.3053434141298723</v>
       </c>
     </row>
     <row r="86" spans="1:5">
@@ -4071,10 +4065,10 @@
         <v>632</v>
       </c>
       <c r="D86">
-        <v>0.8794580797107039</v>
+        <v>0.84172641055338</v>
       </c>
       <c r="E86">
-        <v>0.8693559643291786</v>
+        <v>0.9080673719281944</v>
       </c>
     </row>
     <row r="87" spans="1:5">
@@ -4088,10 +4082,10 @@
         <v>379</v>
       </c>
       <c r="D87">
-        <v>0.9137976402428476</v>
+        <v>0.9074655064289524</v>
       </c>
       <c r="E87">
-        <v>0.9710839654119374</v>
+        <v>0.9611459576836122</v>
       </c>
     </row>
     <row r="88" spans="1:5">
@@ -4105,10 +4099,10 @@
         <v>633</v>
       </c>
       <c r="D88">
-        <v>0.8069959077348787</v>
+        <v>0.7286322791383084</v>
       </c>
       <c r="E88">
-        <v>0.8967992913678643</v>
+        <v>0.8365604171813321</v>
       </c>
     </row>
     <row r="89" spans="1:5">
@@ -4122,10 +4116,10 @@
         <v>634</v>
       </c>
       <c r="D89">
-        <v>0.4882226864478894</v>
+        <v>0.5588419834444958</v>
       </c>
       <c r="E89">
-        <v>0.4378830378440979</v>
+        <v>0.5003156450138365</v>
       </c>
     </row>
     <row r="90" spans="1:5">
@@ -4139,10 +4133,10 @@
         <v>635</v>
       </c>
       <c r="D90">
-        <v>0.7613027949324774</v>
+        <v>0.7584637888358261</v>
       </c>
       <c r="E90">
-        <v>0.7062137249150418</v>
+        <v>0.8670236071988627</v>
       </c>
     </row>
     <row r="91" spans="1:5">
@@ -4156,10 +4150,10 @@
         <v>636</v>
       </c>
       <c r="D91">
-        <v>0.7911982143320918</v>
+        <v>0.8639328364462658</v>
       </c>
       <c r="E91">
-        <v>0.8845913583654457</v>
+        <v>0.942004362113952</v>
       </c>
     </row>
     <row r="92" spans="1:5">
@@ -4172,12 +4166,6 @@
       <c r="C92" t="s">
         <v>637</v>
       </c>
-      <c r="D92">
-        <v>0.3954054258355558</v>
-      </c>
-      <c r="E92">
-        <v>0.5825064019491268</v>
-      </c>
     </row>
     <row r="93" spans="1:5">
       <c r="A93" t="s">
@@ -4189,12 +4177,6 @@
       <c r="C93" t="s">
         <v>638</v>
       </c>
-      <c r="D93">
-        <v>0.6483559519883222</v>
-      </c>
-      <c r="E93">
-        <v>0.5190500965790732</v>
-      </c>
     </row>
     <row r="94" spans="1:5">
       <c r="A94" t="s">
@@ -4207,10 +4189,10 @@
         <v>386</v>
       </c>
       <c r="D94">
-        <v>0.9164336814760163</v>
+        <v>0.8968536000187578</v>
       </c>
       <c r="E94">
-        <v>0.9796849795643681</v>
+        <v>0.956271433243593</v>
       </c>
     </row>
     <row r="95" spans="1:5">
@@ -4224,10 +4206,10 @@
         <v>639</v>
       </c>
       <c r="D95">
-        <v>0.918723235065203</v>
+        <v>0.9334031204725691</v>
       </c>
       <c r="E95">
-        <v>0.9765649388515734</v>
+        <v>0.9875032825797173</v>
       </c>
     </row>
     <row r="96" spans="1:5">
@@ -4241,10 +4223,10 @@
         <v>640</v>
       </c>
       <c r="D96">
-        <v>0.7784015019266604</v>
+        <v>0.8057877459901494</v>
       </c>
       <c r="E96">
-        <v>0.782503387957848</v>
+        <v>0.9200028930809734</v>
       </c>
     </row>
     <row r="97" spans="1:5">
@@ -4258,10 +4240,10 @@
         <v>389</v>
       </c>
       <c r="D97">
-        <v>0.7813775603811834</v>
+        <v>0.8211909497143021</v>
       </c>
       <c r="E97">
-        <v>0.8456132780943261</v>
+        <v>0.9656821151072836</v>
       </c>
     </row>
     <row r="98" spans="1:5">
@@ -4275,10 +4257,10 @@
         <v>641</v>
       </c>
       <c r="D98">
-        <v>0.9702624424953409</v>
+        <v>0.9689911419361753</v>
       </c>
       <c r="E98">
-        <v>0.9851833319431098</v>
+        <v>0.9642719404875445</v>
       </c>
     </row>
     <row r="99" spans="1:5">
@@ -4292,10 +4274,10 @@
         <v>642</v>
       </c>
       <c r="D99">
-        <v>0.9506406756745953</v>
+        <v>0.9320193830384518</v>
       </c>
       <c r="E99">
-        <v>0.9877079033299989</v>
+        <v>0.9645798542884304</v>
       </c>
     </row>
     <row r="100" spans="1:5">
@@ -4309,10 +4291,10 @@
         <v>643</v>
       </c>
       <c r="D100">
-        <v>0.9226717626878113</v>
+        <v>0.8857700179116386</v>
       </c>
       <c r="E100">
-        <v>0.980883791393042</v>
+        <v>0.9373264525331524</v>
       </c>
     </row>
     <row r="101" spans="1:5">
@@ -4326,10 +4308,10 @@
         <v>644</v>
       </c>
       <c r="D101">
-        <v>0.9358669977813112</v>
+        <v>0.9105771251288572</v>
       </c>
       <c r="E101">
-        <v>0.9688421174822137</v>
+        <v>0.9468440295363552</v>
       </c>
     </row>
     <row r="102" spans="1:5">
@@ -4343,10 +4325,10 @@
         <v>394</v>
       </c>
       <c r="D102">
-        <v>0.9523567896449913</v>
+        <v>0.9576460663142904</v>
       </c>
       <c r="E102">
-        <v>0.9922795008831952</v>
+        <v>0.9864826948229924</v>
       </c>
     </row>
     <row r="103" spans="1:5">
@@ -4360,10 +4342,10 @@
         <v>645</v>
       </c>
       <c r="D103">
-        <v>0.8893139616158474</v>
+        <v>0.9007800322579432</v>
       </c>
       <c r="E103">
-        <v>0.7625700803585671</v>
+        <v>0.9722898413393004</v>
       </c>
     </row>
     <row r="104" spans="1:5">
@@ -4377,10 +4359,10 @@
         <v>646</v>
       </c>
       <c r="D104">
-        <v>0.4584919517377998</v>
+        <v>0.6016960609429114</v>
       </c>
       <c r="E104">
-        <v>0.7495657299476869</v>
+        <v>0.6486343131907959</v>
       </c>
     </row>
     <row r="105" spans="1:5">
@@ -4394,10 +4376,10 @@
         <v>647</v>
       </c>
       <c r="D105">
-        <v>0.836579783686053</v>
+        <v>0.8836099155953703</v>
       </c>
       <c r="E105">
-        <v>0.8850967738204997</v>
+        <v>0.8863143793283104</v>
       </c>
     </row>
     <row r="106" spans="1:5">
@@ -4411,10 +4393,10 @@
         <v>648</v>
       </c>
       <c r="D106">
-        <v>0.7756925218228217</v>
+        <v>0.8248947644382093</v>
       </c>
       <c r="E106">
-        <v>0.6590573347896609</v>
+        <v>0.8729495057044838</v>
       </c>
     </row>
     <row r="107" spans="1:5">
@@ -4428,10 +4410,10 @@
         <v>649</v>
       </c>
       <c r="D107">
-        <v>0.7347017753614741</v>
+        <v>0.7750570378731805</v>
       </c>
       <c r="E107">
-        <v>0.7613799512883092</v>
+        <v>0.9175511840975829</v>
       </c>
     </row>
     <row r="108" spans="1:5">
@@ -4445,10 +4427,10 @@
         <v>400</v>
       </c>
       <c r="D108">
-        <v>0.9484595749827408</v>
+        <v>0.9633505520855214</v>
       </c>
       <c r="E108">
-        <v>0.9721690243831</v>
+        <v>0.9657380644205005</v>
       </c>
     </row>
     <row r="109" spans="1:5">
@@ -4462,10 +4444,10 @@
         <v>650</v>
       </c>
       <c r="D109">
-        <v>0.8991545326787629</v>
+        <v>0.8369388018369418</v>
       </c>
       <c r="E109">
-        <v>0.9411521161006396</v>
+        <v>0.9197418545828182</v>
       </c>
     </row>
     <row r="110" spans="1:5">
@@ -4479,10 +4461,10 @@
         <v>651</v>
       </c>
       <c r="D110">
-        <v>0.8033240478559953</v>
+        <v>0.8318949860815466</v>
       </c>
       <c r="E110">
-        <v>0.8124333904601013</v>
+        <v>0.9344668696342397</v>
       </c>
     </row>
     <row r="111" spans="1:5">
@@ -4496,10 +4478,10 @@
         <v>652</v>
       </c>
       <c r="D111">
-        <v>0.7325316894993649</v>
+        <v>0.7421117113320946</v>
       </c>
       <c r="E111">
-        <v>0.6542238738723055</v>
+        <v>0.6812009724720619</v>
       </c>
     </row>
     <row r="112" spans="1:5">
@@ -4513,10 +4495,10 @@
         <v>404</v>
       </c>
       <c r="D112">
-        <v>0.7826219563865584</v>
+        <v>0.8866491470308466</v>
       </c>
       <c r="E112">
-        <v>0.9410170774518862</v>
+        <v>0.7652024833941766</v>
       </c>
     </row>
     <row r="113" spans="1:5">
@@ -4530,10 +4512,10 @@
         <v>653</v>
       </c>
       <c r="D113">
-        <v>0.8664314395760876</v>
+        <v>0.7964737333895289</v>
       </c>
       <c r="E113">
-        <v>0.8965628214568073</v>
+        <v>0.9278977500940708</v>
       </c>
     </row>
     <row r="114" spans="1:5">
@@ -4547,10 +4529,10 @@
         <v>654</v>
       </c>
       <c r="D114">
-        <v>0.6670762577726477</v>
+        <v>0.6116454712464048</v>
       </c>
       <c r="E114">
-        <v>0.4679330773716387</v>
+        <v>0.3645856826102471</v>
       </c>
     </row>
     <row r="115" spans="1:5">
@@ -4564,10 +4546,10 @@
         <v>407</v>
       </c>
       <c r="D115">
-        <v>0.9389363030599504</v>
+        <v>0.9507064150612218</v>
       </c>
       <c r="E115">
-        <v>0.9932502143950912</v>
+        <v>0.9841465719154012</v>
       </c>
     </row>
     <row r="116" spans="1:5">
@@ -4581,10 +4563,10 @@
         <v>408</v>
       </c>
       <c r="D116">
-        <v>0.946277833396851</v>
+        <v>0.8954626798444519</v>
       </c>
       <c r="E116">
-        <v>0.9753867415564452</v>
+        <v>0.9173094797189858</v>
       </c>
     </row>
     <row r="117" spans="1:5">
@@ -4598,10 +4580,10 @@
         <v>655</v>
       </c>
       <c r="D117">
-        <v>0.9678807630363566</v>
+        <v>0.9835847805350825</v>
       </c>
       <c r="E117">
-        <v>0.9917697725937413</v>
+        <v>0.996697523258859</v>
       </c>
     </row>
     <row r="118" spans="1:5">
@@ -4615,10 +4597,10 @@
         <v>410</v>
       </c>
       <c r="D118">
-        <v>0.3755157504513215</v>
+        <v>0.3055722219249775</v>
       </c>
       <c r="E118">
-        <v>0.3585908250956003</v>
+        <v>0.5807020629633469</v>
       </c>
     </row>
     <row r="119" spans="1:5">
@@ -4632,10 +4614,10 @@
         <v>411</v>
       </c>
       <c r="D119">
-        <v>0.3544869634538582</v>
+        <v>0.5127073031515079</v>
       </c>
       <c r="E119">
-        <v>0.08483447753182145</v>
+        <v>0.1886511745202985</v>
       </c>
     </row>
     <row r="120" spans="1:5">
@@ -4649,10 +4631,10 @@
         <v>656</v>
       </c>
       <c r="D120">
-        <v>0.2469973195478499</v>
+        <v>0.2612902525557634</v>
       </c>
       <c r="E120">
-        <v>0.22265256663717</v>
+        <v>0.2775316855615095</v>
       </c>
     </row>
     <row r="121" spans="1:5">
@@ -4666,10 +4648,10 @@
         <v>413</v>
       </c>
       <c r="D121">
-        <v>0.7823283256222264</v>
+        <v>0.8035007254211293</v>
       </c>
       <c r="E121">
-        <v>0.8958705674173567</v>
+        <v>0.715843927697584</v>
       </c>
     </row>
     <row r="122" spans="1:5">
@@ -4683,10 +4665,10 @@
         <v>657</v>
       </c>
       <c r="D122">
-        <v>0.7789422105945366</v>
+        <v>0.7384964327946595</v>
       </c>
       <c r="E122">
-        <v>0.9133861586901291</v>
+        <v>0.9093089269525418</v>
       </c>
     </row>
     <row r="123" spans="1:5">
@@ -4700,10 +4682,10 @@
         <v>415</v>
       </c>
       <c r="D123">
-        <v>0.6135295012414999</v>
+        <v>0.5418212175335672</v>
       </c>
       <c r="E123">
-        <v>0.6324917426369753</v>
+        <v>0.5903669022906618</v>
       </c>
     </row>
     <row r="124" spans="1:5">
@@ -4717,10 +4699,10 @@
         <v>416</v>
       </c>
       <c r="D124">
-        <v>0.4149956681092521</v>
+        <v>0.352924947718529</v>
       </c>
       <c r="E124">
-        <v>0.2554520706648434</v>
+        <v>0.2603309207090556</v>
       </c>
     </row>
     <row r="125" spans="1:5">
@@ -4734,10 +4716,10 @@
         <v>658</v>
       </c>
       <c r="D125">
-        <v>0.8431843193331912</v>
+        <v>0.8147711351928278</v>
       </c>
       <c r="E125">
-        <v>0.9165574029753787</v>
+        <v>0.8936727431256929</v>
       </c>
     </row>
     <row r="126" spans="1:5">
@@ -4751,10 +4733,10 @@
         <v>418</v>
       </c>
       <c r="D126">
-        <v>0.8495153431236153</v>
+        <v>0.9088771549334178</v>
       </c>
       <c r="E126">
-        <v>0.9623752166338416</v>
+        <v>0.96455872499482</v>
       </c>
     </row>
     <row r="127" spans="1:5">
@@ -4768,10 +4750,10 @@
         <v>419</v>
       </c>
       <c r="D127">
-        <v>0.4613630238479765</v>
+        <v>0.5485253737989056</v>
       </c>
       <c r="E127">
-        <v>0.1703673879302488</v>
+        <v>0.3127630083184071</v>
       </c>
     </row>
     <row r="128" spans="1:5">
@@ -4785,10 +4767,10 @@
         <v>659</v>
       </c>
       <c r="D128">
-        <v>0.7940011666507344</v>
+        <v>0.7969099871442281</v>
       </c>
       <c r="E128">
-        <v>0.9195983747983604</v>
+        <v>0.8880863784999057</v>
       </c>
     </row>
     <row r="129" spans="1:5">
@@ -4802,10 +4784,10 @@
         <v>660</v>
       </c>
       <c r="D129">
-        <v>0.9155771895607711</v>
+        <v>0.8340559702352421</v>
       </c>
       <c r="E129">
-        <v>0.9674752008694604</v>
+        <v>0.9248035881028526</v>
       </c>
     </row>
     <row r="130" spans="1:5">
@@ -4819,10 +4801,10 @@
         <v>661</v>
       </c>
       <c r="D130">
-        <v>0.3518286859803335</v>
+        <v>0.645944378611761</v>
       </c>
       <c r="E130">
-        <v>0.425690384377267</v>
+        <v>0.8134744987404906</v>
       </c>
     </row>
     <row r="131" spans="1:5">
@@ -4836,10 +4818,10 @@
         <v>423</v>
       </c>
       <c r="D131">
-        <v>0.7432761709791702</v>
+        <v>0.7008738250183071</v>
       </c>
       <c r="E131">
-        <v>0.6112252011671442</v>
+        <v>0.5337807105703778</v>
       </c>
     </row>
     <row r="132" spans="1:5">
@@ -4853,10 +4835,10 @@
         <v>662</v>
       </c>
       <c r="D132">
-        <v>0.4995059645412618</v>
+        <v>0.4049953490565011</v>
       </c>
       <c r="E132">
-        <v>0.3004881390873814</v>
+        <v>0.3151049564350391</v>
       </c>
     </row>
     <row r="133" spans="1:5">
@@ -4870,10 +4852,10 @@
         <v>425</v>
       </c>
       <c r="D133">
-        <v>0.8709344831472219</v>
+        <v>0.8342538666454506</v>
       </c>
       <c r="E133">
-        <v>0.8681055618231324</v>
+        <v>0.7958451539863018</v>
       </c>
     </row>
     <row r="134" spans="1:5">
@@ -4887,10 +4869,10 @@
         <v>426</v>
       </c>
       <c r="D134">
-        <v>0.6621996845242963</v>
+        <v>0.6190353663167099</v>
       </c>
       <c r="E134">
-        <v>0.452174668318409</v>
+        <v>0.5263683082025595</v>
       </c>
     </row>
     <row r="135" spans="1:5">
@@ -4904,10 +4886,10 @@
         <v>427</v>
       </c>
       <c r="D135">
-        <v>0.7101555463364005</v>
+        <v>0.6470677699708022</v>
       </c>
       <c r="E135">
-        <v>0.8079534767314602</v>
+        <v>0.8408602091715028</v>
       </c>
     </row>
     <row r="136" spans="1:5">
@@ -4920,12 +4902,6 @@
       <c r="C136" t="s">
         <v>663</v>
       </c>
-      <c r="D136">
-        <v>0.5521111212441183</v>
-      </c>
-      <c r="E136">
-        <v>0.684967710049826</v>
-      </c>
     </row>
     <row r="137" spans="1:5">
       <c r="A137" t="s">
@@ -4938,10 +4914,10 @@
         <v>664</v>
       </c>
       <c r="D137">
-        <v>0.2813466745361016</v>
+        <v>0.3561696164960642</v>
       </c>
       <c r="E137">
-        <v>0.07618857089831511</v>
+        <v>0.4021088114002869</v>
       </c>
     </row>
     <row r="138" spans="1:5">
@@ -4955,10 +4931,10 @@
         <v>665</v>
       </c>
       <c r="D138">
-        <v>0.7625745125721078</v>
+        <v>0.5677104020915339</v>
       </c>
       <c r="E138">
-        <v>0.8124530021939127</v>
+        <v>0.821744763260123</v>
       </c>
     </row>
     <row r="139" spans="1:5">
@@ -4972,10 +4948,10 @@
         <v>431</v>
       </c>
       <c r="D139">
-        <v>0.9461256308954294</v>
+        <v>0.964371356688728</v>
       </c>
       <c r="E139">
-        <v>0.9596106595287264</v>
+        <v>0.9880314050092553</v>
       </c>
     </row>
     <row r="140" spans="1:5">
@@ -4989,10 +4965,10 @@
         <v>666</v>
       </c>
       <c r="D140">
-        <v>0.3580108056269704</v>
+        <v>0.3168344798293073</v>
       </c>
       <c r="E140">
-        <v>0.2565142386649095</v>
+        <v>0.2055126122049565</v>
       </c>
     </row>
     <row r="141" spans="1:5">
@@ -5006,10 +4982,10 @@
         <v>433</v>
       </c>
       <c r="D141">
-        <v>0.9859069501640985</v>
+        <v>0.9915334622063405</v>
       </c>
       <c r="E141">
-        <v>0.9990126080282103</v>
+        <v>0.9943221638976657</v>
       </c>
     </row>
     <row r="142" spans="1:5">
@@ -5023,10 +4999,10 @@
         <v>667</v>
       </c>
       <c r="D142">
-        <v>0.9378326586733291</v>
+        <v>0.9408547101014759</v>
       </c>
       <c r="E142">
-        <v>0.9695738013097548</v>
+        <v>0.9726584140974417</v>
       </c>
     </row>
     <row r="143" spans="1:5">
@@ -5040,10 +5016,10 @@
         <v>435</v>
       </c>
       <c r="D143">
-        <v>0.9159742936291253</v>
+        <v>0.9049503948318606</v>
       </c>
       <c r="E143">
-        <v>0.9565132202658311</v>
+        <v>0.9520085853454848</v>
       </c>
     </row>
     <row r="144" spans="1:5">
@@ -5057,10 +5033,10 @@
         <v>668</v>
       </c>
       <c r="D144">
-        <v>0.6014988457429379</v>
+        <v>0.6975578773103706</v>
       </c>
       <c r="E144">
-        <v>0.5648602446742017</v>
+        <v>0.5154546279883463</v>
       </c>
     </row>
     <row r="145" spans="1:5">
@@ -5074,10 +5050,10 @@
         <v>437</v>
       </c>
       <c r="D145">
-        <v>0.9020262819389147</v>
+        <v>0.9492793439415675</v>
       </c>
       <c r="E145">
-        <v>0.9795031157409593</v>
+        <v>0.9652929806520902</v>
       </c>
     </row>
     <row r="146" spans="1:5">
@@ -5091,10 +5067,10 @@
         <v>669</v>
       </c>
       <c r="D146">
-        <v>0.7048569325894561</v>
+        <v>0.6849100723834848</v>
       </c>
       <c r="E146">
-        <v>0.5171515681656828</v>
+        <v>0.5696156711489806</v>
       </c>
     </row>
     <row r="147" spans="1:5">
@@ -5108,10 +5084,10 @@
         <v>670</v>
       </c>
       <c r="D147">
-        <v>0.4735832393528591</v>
+        <v>0.3580530766544792</v>
       </c>
       <c r="E147">
-        <v>0.3988860459014134</v>
+        <v>0.343469340432244</v>
       </c>
     </row>
     <row r="148" spans="1:5">
@@ -5125,10 +5101,10 @@
         <v>440</v>
       </c>
       <c r="D148">
-        <v>0.5457123144632606</v>
+        <v>0.6787180386694198</v>
       </c>
       <c r="E148">
-        <v>0.1354787508389723</v>
+        <v>0.1613625310760468</v>
       </c>
     </row>
     <row r="149" spans="1:5">
@@ -5142,10 +5118,10 @@
         <v>671</v>
       </c>
       <c r="D149">
-        <v>0.7850867903466474</v>
+        <v>0.8143484682072152</v>
       </c>
       <c r="E149">
-        <v>0.9604392757244987</v>
+        <v>0.8663432006935127</v>
       </c>
     </row>
     <row r="150" spans="1:5">
@@ -5159,10 +5135,10 @@
         <v>672</v>
       </c>
       <c r="D150">
-        <v>0.9122475017831416</v>
+        <v>0.9011989817973378</v>
       </c>
       <c r="E150">
-        <v>0.954229100337877</v>
+        <v>0.9823212407641354</v>
       </c>
     </row>
     <row r="151" spans="1:5">
@@ -5176,10 +5152,10 @@
         <v>673</v>
       </c>
       <c r="D151">
-        <v>0.8661064496339093</v>
+        <v>0.8773874077114825</v>
       </c>
       <c r="E151">
-        <v>0.8996079236055121</v>
+        <v>0.8454004233619281</v>
       </c>
     </row>
     <row r="152" spans="1:5">
@@ -5193,10 +5169,10 @@
         <v>674</v>
       </c>
       <c r="D152">
-        <v>0.5099175807056365</v>
+        <v>0.3937974422475622</v>
       </c>
       <c r="E152">
-        <v>0.6412028002100384</v>
+        <v>0.5022655532984401</v>
       </c>
     </row>
     <row r="153" spans="1:5">
@@ -5210,10 +5186,10 @@
         <v>675</v>
       </c>
       <c r="D153">
-        <v>0.9545764341891024</v>
+        <v>0.9634418208738091</v>
       </c>
       <c r="E153">
-        <v>0.9897139913115892</v>
+        <v>0.9915604222646374</v>
       </c>
     </row>
     <row r="154" spans="1:5">
@@ -5227,10 +5203,10 @@
         <v>676</v>
       </c>
       <c r="D154">
-        <v>0.5728015600280393</v>
+        <v>0.615791133536049</v>
       </c>
       <c r="E154">
-        <v>0.8287607100066439</v>
+        <v>0.521110513778389</v>
       </c>
     </row>
     <row r="155" spans="1:5">
@@ -5244,10 +5220,10 @@
         <v>447</v>
       </c>
       <c r="D155">
-        <v>0.8120832034268303</v>
+        <v>0.7541809361145346</v>
       </c>
       <c r="E155">
-        <v>0.7820523452356799</v>
+        <v>0.849774264375102</v>
       </c>
     </row>
     <row r="156" spans="1:5">
@@ -5261,10 +5237,10 @@
         <v>448</v>
       </c>
       <c r="D156">
-        <v>0.5614501417974735</v>
+        <v>0.510861696862953</v>
       </c>
       <c r="E156">
-        <v>0.304260112408232</v>
+        <v>0.2588224971224633</v>
       </c>
     </row>
     <row r="157" spans="1:5">
@@ -5278,10 +5254,10 @@
         <v>677</v>
       </c>
       <c r="D157">
-        <v>0.687742675279043</v>
+        <v>0.7132536217343323</v>
       </c>
       <c r="E157">
-        <v>0.8687815787781417</v>
+        <v>0.8913663341229745</v>
       </c>
     </row>
     <row r="158" spans="1:5">
@@ -5295,10 +5271,10 @@
         <v>450</v>
       </c>
       <c r="D158">
-        <v>0.7710405636884624</v>
+        <v>0.798509783276476</v>
       </c>
       <c r="E158">
-        <v>0.7657398608840466</v>
+        <v>0.8019725291913485</v>
       </c>
     </row>
     <row r="159" spans="1:5">
@@ -5312,10 +5288,10 @@
         <v>678</v>
       </c>
       <c r="D159">
-        <v>0.5589354205409214</v>
+        <v>0.7124970133322126</v>
       </c>
       <c r="E159">
-        <v>0.5416352430018776</v>
+        <v>0.6547824080100697</v>
       </c>
     </row>
     <row r="160" spans="1:5">
@@ -5329,10 +5305,10 @@
         <v>679</v>
       </c>
       <c r="D160">
-        <v>0.9585309421493973</v>
+        <v>0.9641454274554637</v>
       </c>
       <c r="E160">
-        <v>0.9436790836634765</v>
+        <v>0.9900246959555041</v>
       </c>
     </row>
     <row r="161" spans="1:5">
@@ -5346,10 +5322,10 @@
         <v>453</v>
       </c>
       <c r="D161">
-        <v>0.6434045416223402</v>
+        <v>0.7088884892634357</v>
       </c>
       <c r="E161">
-        <v>0.799198419289151</v>
+        <v>0.7473491139691463</v>
       </c>
     </row>
     <row r="162" spans="1:5">
@@ -5363,10 +5339,10 @@
         <v>680</v>
       </c>
       <c r="D162">
-        <v>0.375541258274233</v>
+        <v>0.2084069812135467</v>
       </c>
       <c r="E162">
-        <v>0.2382211330810547</v>
+        <v>0.2540216834184071</v>
       </c>
     </row>
     <row r="163" spans="1:5">
@@ -5380,10 +5356,10 @@
         <v>455</v>
       </c>
       <c r="D163">
-        <v>0.9467337589387799</v>
+        <v>0.9577110076403419</v>
       </c>
       <c r="E163">
-        <v>0.9942546053310508</v>
+        <v>0.9915675652266078</v>
       </c>
     </row>
     <row r="164" spans="1:5">
@@ -5397,10 +5373,10 @@
         <v>456</v>
       </c>
       <c r="D164">
-        <v>0.315260144290982</v>
+        <v>0.3044137052638726</v>
       </c>
       <c r="E164">
-        <v>0.532229123251337</v>
+        <v>0.3244043536473521</v>
       </c>
     </row>
     <row r="165" spans="1:5">
@@ -5414,10 +5390,10 @@
         <v>457</v>
       </c>
       <c r="D165">
-        <v>0.5007340497268655</v>
+        <v>0.5532352239258298</v>
       </c>
       <c r="E165">
-        <v>0.3442704045523785</v>
+        <v>0.7130600759303539</v>
       </c>
     </row>
     <row r="166" spans="1:5">
@@ -5431,10 +5407,10 @@
         <v>458</v>
       </c>
       <c r="D166">
-        <v>0.6821156963159299</v>
+        <v>0.6513524907852029</v>
       </c>
       <c r="E166">
-        <v>0.6950807711687057</v>
+        <v>0.6274228658646749</v>
       </c>
     </row>
     <row r="167" spans="1:5">
@@ -5448,10 +5424,10 @@
         <v>459</v>
       </c>
       <c r="D167">
-        <v>0.7509101702025699</v>
+        <v>0.7209116370133988</v>
       </c>
       <c r="E167">
-        <v>0.7062833686000757</v>
+        <v>0.5723168016879826</v>
       </c>
     </row>
     <row r="168" spans="1:5">
@@ -5465,10 +5441,10 @@
         <v>681</v>
       </c>
       <c r="D168">
-        <v>0.8482746576353805</v>
+        <v>0.8280829215537225</v>
       </c>
       <c r="E168">
-        <v>0.9039891392301637</v>
+        <v>0.9014892100094551</v>
       </c>
     </row>
     <row r="169" spans="1:5">
@@ -5482,10 +5458,10 @@
         <v>461</v>
       </c>
       <c r="D169">
-        <v>0.8377333029075936</v>
+        <v>0.6677167438629862</v>
       </c>
       <c r="E169">
-        <v>0.6811327037604492</v>
+        <v>0.6663992800964182</v>
       </c>
     </row>
     <row r="170" spans="1:5">
@@ -5499,10 +5475,10 @@
         <v>682</v>
       </c>
       <c r="D170">
-        <v>0.838490839654719</v>
+        <v>0.7967827194791056</v>
       </c>
       <c r="E170">
-        <v>0.8202214795335528</v>
+        <v>0.757083516219862</v>
       </c>
     </row>
     <row r="171" spans="1:5">
@@ -5516,10 +5492,10 @@
         <v>683</v>
       </c>
       <c r="D171">
-        <v>0.7621947673118828</v>
+        <v>0.7990421474813212</v>
       </c>
       <c r="E171">
-        <v>0.8135358004183121</v>
+        <v>0.8912648136903677</v>
       </c>
     </row>
     <row r="172" spans="1:5">
@@ -5533,10 +5509,10 @@
         <v>684</v>
       </c>
       <c r="D172">
-        <v>0.8209946307506649</v>
+        <v>0.850471850284684</v>
       </c>
       <c r="E172">
-        <v>0.8836100079454428</v>
+        <v>0.9374094016368273</v>
       </c>
     </row>
     <row r="173" spans="1:5">
@@ -5550,10 +5526,10 @@
         <v>685</v>
       </c>
       <c r="D173">
-        <v>0.848083409671213</v>
+        <v>0.8482519565358767</v>
       </c>
       <c r="E173">
-        <v>0.9077466701632172</v>
+        <v>0.865447764782488</v>
       </c>
     </row>
     <row r="174" spans="1:5">
@@ -5567,10 +5543,10 @@
         <v>466</v>
       </c>
       <c r="D174">
-        <v>0.8514428600476698</v>
+        <v>0.9507815075891534</v>
       </c>
       <c r="E174">
-        <v>0.966431941757251</v>
+        <v>0.9414785096648882</v>
       </c>
     </row>
     <row r="175" spans="1:5">
@@ -5584,10 +5560,10 @@
         <v>467</v>
       </c>
       <c r="D175">
-        <v>0.6366433982402167</v>
+        <v>0.6084802923294518</v>
       </c>
       <c r="E175">
-        <v>0.7841896055109148</v>
+        <v>0.6214451313226921</v>
       </c>
     </row>
     <row r="176" spans="1:5">
@@ -5601,10 +5577,10 @@
         <v>468</v>
       </c>
       <c r="D176">
-        <v>0.5887670135649953</v>
+        <v>0.5429799092102551</v>
       </c>
       <c r="E176">
-        <v>0.5545394289243997</v>
+        <v>0.4623052379527183</v>
       </c>
     </row>
     <row r="177" spans="1:5">
@@ -5617,12 +5593,6 @@
       <c r="C177" t="s">
         <v>469</v>
       </c>
-      <c r="D177">
-        <v>0.5627489935460889</v>
-      </c>
-      <c r="E177">
-        <v>0.5990555464690608</v>
-      </c>
     </row>
     <row r="178" spans="1:5">
       <c r="A178" t="s">
@@ -5635,10 +5605,10 @@
         <v>470</v>
       </c>
       <c r="D178">
-        <v>0.821822646781026</v>
+        <v>0.8666979257493425</v>
       </c>
       <c r="E178">
-        <v>0.8885233806590002</v>
+        <v>0.9420667234342637</v>
       </c>
     </row>
     <row r="179" spans="1:5">
@@ -5652,10 +5622,10 @@
         <v>471</v>
       </c>
       <c r="D179">
-        <v>0.8315096108399993</v>
+        <v>0.911081448701109</v>
       </c>
       <c r="E179">
-        <v>0.9047513698164841</v>
+        <v>0.9688189827322214</v>
       </c>
     </row>
     <row r="180" spans="1:5">
@@ -5669,10 +5639,10 @@
         <v>472</v>
       </c>
       <c r="D180">
-        <v>0.9060482293455026</v>
+        <v>0.8712017354130697</v>
       </c>
       <c r="E180">
-        <v>0.9554945057471349</v>
+        <v>0.9630306947546017</v>
       </c>
     </row>
     <row r="181" spans="1:5">
@@ -5686,10 +5656,10 @@
         <v>686</v>
       </c>
       <c r="D181">
-        <v>0.675878497315378</v>
+        <v>0.6193452764645382</v>
       </c>
       <c r="E181">
-        <v>0.7877793776152301</v>
+        <v>0.8430589868505756</v>
       </c>
     </row>
     <row r="182" spans="1:5">
@@ -5703,10 +5673,10 @@
         <v>474</v>
       </c>
       <c r="D182">
-        <v>0.9031981658130337</v>
+        <v>0.9187957229047415</v>
       </c>
       <c r="E182">
-        <v>0.9178827112081672</v>
+        <v>0.9482442601383804</v>
       </c>
     </row>
     <row r="183" spans="1:5">
@@ -5720,10 +5690,10 @@
         <v>687</v>
       </c>
       <c r="D183">
-        <v>0.1859965467595384</v>
+        <v>0.1252523649577434</v>
       </c>
       <c r="E183">
-        <v>0.09967312891147657</v>
+        <v>0.04894008199600303</v>
       </c>
     </row>
     <row r="184" spans="1:5">
@@ -5737,10 +5707,10 @@
         <v>476</v>
       </c>
       <c r="D184">
-        <v>0.09598546935979248</v>
+        <v>0.1177345203264332</v>
       </c>
       <c r="E184">
-        <v>0.0963513674135722</v>
+        <v>0.06183535586890299</v>
       </c>
     </row>
     <row r="185" spans="1:5">
@@ -5754,10 +5724,10 @@
         <v>477</v>
       </c>
       <c r="D185">
-        <v>0.2777138888754705</v>
+        <v>0.3213299093420761</v>
       </c>
       <c r="E185">
-        <v>0.5764039518611551</v>
+        <v>0.4487612144474164</v>
       </c>
     </row>
     <row r="186" spans="1:5">
@@ -5771,10 +5741,10 @@
         <v>470</v>
       </c>
       <c r="D186">
-        <v>0.9287486386502387</v>
+        <v>0.9351815868118077</v>
       </c>
       <c r="E186">
-        <v>0.9756297316782976</v>
+        <v>0.9789760410010233</v>
       </c>
     </row>
     <row r="187" spans="1:5">
@@ -5788,10 +5758,10 @@
         <v>688</v>
       </c>
       <c r="D187">
-        <v>0.7672915144366644</v>
+        <v>0.844062296448236</v>
       </c>
       <c r="E187">
-        <v>0.9406644421026464</v>
+        <v>0.9132197599321897</v>
       </c>
     </row>
     <row r="188" spans="1:5">
@@ -5805,10 +5775,10 @@
         <v>689</v>
       </c>
       <c r="D188">
-        <v>0.7886111577430811</v>
+        <v>0.864666838183952</v>
       </c>
       <c r="E188">
-        <v>0.902225629547646</v>
+        <v>0.9198448467677569</v>
       </c>
     </row>
     <row r="189" spans="1:5">
@@ -5822,10 +5792,10 @@
         <v>481</v>
       </c>
       <c r="D189">
-        <v>0.8515673365221089</v>
+        <v>0.8806437417470697</v>
       </c>
       <c r="E189">
-        <v>0.9693822277558652</v>
+        <v>0.9667932332298242</v>
       </c>
     </row>
     <row r="190" spans="1:5">
@@ -5839,10 +5809,10 @@
         <v>482</v>
       </c>
       <c r="D190">
-        <v>0.8393826894399977</v>
+        <v>0.7759211514843412</v>
       </c>
       <c r="E190">
-        <v>0.9066683744564162</v>
+        <v>0.7801262084804218</v>
       </c>
     </row>
     <row r="191" spans="1:5">
@@ -5856,10 +5826,10 @@
         <v>690</v>
       </c>
       <c r="D191">
-        <v>0.4976791761031745</v>
+        <v>0.6934321796587749</v>
       </c>
       <c r="E191">
-        <v>0.3159148093718885</v>
+        <v>0.7302764979803821</v>
       </c>
     </row>
     <row r="192" spans="1:5">
@@ -5873,10 +5843,10 @@
         <v>691</v>
       </c>
       <c r="D192">
-        <v>0.9584536694740503</v>
+        <v>0.9448215439847975</v>
       </c>
       <c r="E192">
-        <v>0.9786033822773755</v>
+        <v>0.922668041648955</v>
       </c>
     </row>
     <row r="193" spans="1:5">
@@ -5890,10 +5860,10 @@
         <v>485</v>
       </c>
       <c r="D193">
-        <v>0.970478622998717</v>
+        <v>0.9763048888727655</v>
       </c>
       <c r="E193">
-        <v>0.9965720264578952</v>
+        <v>0.9921454846804707</v>
       </c>
     </row>
     <row r="194" spans="1:5">
@@ -5906,12 +5876,6 @@
       <c r="C194" t="s">
         <v>692</v>
       </c>
-      <c r="D194">
-        <v>0.7846821899179579</v>
-      </c>
-      <c r="E194">
-        <v>0.7751509865856756</v>
-      </c>
     </row>
     <row r="195" spans="1:5">
       <c r="A195" t="s">
@@ -5924,10 +5888,10 @@
         <v>693</v>
       </c>
       <c r="D195">
-        <v>0.1451409516264554</v>
+        <v>0.1037876291356222</v>
       </c>
       <c r="E195">
-        <v>0.04210762440234288</v>
+        <v>0.05839763334120617</v>
       </c>
     </row>
     <row r="196" spans="1:5">
@@ -5940,12 +5904,6 @@
       <c r="C196" t="s">
         <v>694</v>
       </c>
-      <c r="D196">
-        <v>0.8930976993793974</v>
-      </c>
-      <c r="E196">
-        <v>0.9220475330010015</v>
-      </c>
     </row>
     <row r="197" spans="1:5">
       <c r="A197" t="s">
@@ -5958,10 +5916,10 @@
         <v>489</v>
       </c>
       <c r="D197">
-        <v>0.9224789223820976</v>
+        <v>0.8788278036787635</v>
       </c>
       <c r="E197">
-        <v>0.9747943674311018</v>
+        <v>0.9508514728418564</v>
       </c>
     </row>
     <row r="198" spans="1:5">
@@ -5975,10 +5933,10 @@
         <v>695</v>
       </c>
       <c r="D198">
-        <v>0.8466610161956981</v>
+        <v>0.8390556659249823</v>
       </c>
       <c r="E198">
-        <v>0.8717182619038075</v>
+        <v>0.9278717964493735</v>
       </c>
     </row>
     <row r="199" spans="1:5">
@@ -5992,10 +5950,10 @@
         <v>491</v>
       </c>
       <c r="D199">
-        <v>0.6037667086235992</v>
+        <v>0.4184769556180611</v>
       </c>
       <c r="E199">
-        <v>0.6210942042978359</v>
+        <v>0.5532202565195512</v>
       </c>
     </row>
     <row r="200" spans="1:5">
@@ -6009,10 +5967,10 @@
         <v>696</v>
       </c>
       <c r="D200">
-        <v>0.8750493207673306</v>
+        <v>0.8677644002619259</v>
       </c>
       <c r="E200">
-        <v>0.9558178348290838</v>
+        <v>0.9137747526035482</v>
       </c>
     </row>
     <row r="201" spans="1:5">
@@ -6026,10 +5984,10 @@
         <v>493</v>
       </c>
       <c r="D201">
-        <v>0.8127697923801255</v>
+        <v>0.790116570695053</v>
       </c>
       <c r="E201">
-        <v>0.8233419917975483</v>
+        <v>0.9622412455991753</v>
       </c>
     </row>
     <row r="202" spans="1:5">
@@ -6043,10 +6001,10 @@
         <v>697</v>
       </c>
       <c r="D202">
-        <v>0.8836574652583379</v>
+        <v>0.8686530148154351</v>
       </c>
       <c r="E202">
-        <v>0.9559652022137843</v>
+        <v>0.9156247870349362</v>
       </c>
     </row>
     <row r="203" spans="1:5">
@@ -6059,12 +6017,6 @@
       <c r="C203" t="s">
         <v>495</v>
       </c>
-      <c r="D203">
-        <v>0.6608227117532663</v>
-      </c>
-      <c r="E203">
-        <v>0.6384923506871674</v>
-      </c>
     </row>
     <row r="204" spans="1:5">
       <c r="A204" t="s">
@@ -6077,10 +6029,10 @@
         <v>496</v>
       </c>
       <c r="D204">
-        <v>0.4752698967684498</v>
+        <v>0.4862140132497975</v>
       </c>
       <c r="E204">
-        <v>0.3025904194276152</v>
+        <v>0.6585118317544525</v>
       </c>
     </row>
     <row r="205" spans="1:5">
@@ -6094,10 +6046,10 @@
         <v>497</v>
       </c>
       <c r="D205">
-        <v>0.06530370501075652</v>
+        <v>0.07360844920241286</v>
       </c>
       <c r="E205">
-        <v>0.008187995766205556</v>
+        <v>0.01558703497319515</v>
       </c>
     </row>
     <row r="206" spans="1:5">
@@ -6111,10 +6063,10 @@
         <v>698</v>
       </c>
       <c r="D206">
-        <v>0.593249433129771</v>
+        <v>0.5495298871067493</v>
       </c>
       <c r="E206">
-        <v>0.2635240587222066</v>
+        <v>0.4199428096435817</v>
       </c>
     </row>
     <row r="207" spans="1:5">
@@ -6128,10 +6080,10 @@
         <v>499</v>
       </c>
       <c r="D207">
-        <v>0.8348315528697543</v>
+        <v>0.7955835240566885</v>
       </c>
       <c r="E207">
-        <v>0.6661462670036293</v>
+        <v>0.6507202876533829</v>
       </c>
     </row>
     <row r="208" spans="1:5">
@@ -6145,10 +6097,10 @@
         <v>699</v>
       </c>
       <c r="D208">
-        <v>0.7597942924002533</v>
+        <v>0.9101760511585244</v>
       </c>
       <c r="E208">
-        <v>0.8242143721977835</v>
+        <v>0.9059686679945581</v>
       </c>
     </row>
     <row r="209" spans="1:5">
@@ -6162,10 +6114,10 @@
         <v>501</v>
       </c>
       <c r="D209">
-        <v>0.887372401114382</v>
+        <v>0.8276793602822803</v>
       </c>
       <c r="E209">
-        <v>0.882056454985545</v>
+        <v>0.8760782499875409</v>
       </c>
     </row>
     <row r="210" spans="1:5">
@@ -6179,10 +6131,10 @@
         <v>700</v>
       </c>
       <c r="D210">
-        <v>0.7080492668761122</v>
+        <v>0.7107441079406689</v>
       </c>
       <c r="E210">
-        <v>0.4500142821731583</v>
+        <v>0.7293795633125286</v>
       </c>
     </row>
     <row r="211" spans="1:5">
@@ -6207,10 +6159,10 @@
         <v>701</v>
       </c>
       <c r="D212">
-        <v>0.70000549076454</v>
+        <v>0.8721268655905636</v>
       </c>
       <c r="E212">
-        <v>0.8161213080162897</v>
+        <v>0.8898135912535566</v>
       </c>
     </row>
     <row r="213" spans="1:5">
@@ -6224,10 +6176,10 @@
         <v>505</v>
       </c>
       <c r="D213">
-        <v>0.9777004874428432</v>
+        <v>0.9220541118938267</v>
       </c>
       <c r="E213">
-        <v>0.9952957469139697</v>
+        <v>0.9652049670365623</v>
       </c>
     </row>
     <row r="214" spans="1:5">
@@ -6241,10 +6193,10 @@
         <v>506</v>
       </c>
       <c r="D214">
-        <v>0.9209180650037219</v>
+        <v>0.8745048202224408</v>
       </c>
       <c r="E214">
-        <v>0.9642849280639997</v>
+        <v>0.9692099840871214</v>
       </c>
     </row>
     <row r="215" spans="1:5">
@@ -6258,10 +6210,10 @@
         <v>507</v>
       </c>
       <c r="D215">
-        <v>0.8593815659529305</v>
+        <v>0.9027453627788038</v>
       </c>
       <c r="E215">
-        <v>0.9297090894076994</v>
+        <v>0.9551055832619449</v>
       </c>
     </row>
     <row r="216" spans="1:5">
@@ -6275,10 +6227,10 @@
         <v>702</v>
       </c>
       <c r="D216">
-        <v>0.7860640989795832</v>
+        <v>0.8513519708184686</v>
       </c>
       <c r="E216">
-        <v>0.7580823459180042</v>
+        <v>0.8895986388161434</v>
       </c>
     </row>
     <row r="217" spans="1:5">
@@ -6292,10 +6244,10 @@
         <v>509</v>
       </c>
       <c r="D217">
-        <v>0.8340126933846107</v>
+        <v>0.7049080977586465</v>
       </c>
       <c r="E217">
-        <v>0.8315491423743634</v>
+        <v>0.7663830200705203</v>
       </c>
     </row>
     <row r="218" spans="1:5">
@@ -6309,10 +6261,10 @@
         <v>510</v>
       </c>
       <c r="D218">
-        <v>0.9178465459786839</v>
+        <v>0.8903898263866612</v>
       </c>
       <c r="E218">
-        <v>0.9749761415500943</v>
+        <v>0.944880959093448</v>
       </c>
     </row>
     <row r="219" spans="1:5">
@@ -6326,10 +6278,10 @@
         <v>511</v>
       </c>
       <c r="D219">
-        <v>0.9077266286988538</v>
+        <v>0.8917354318506706</v>
       </c>
       <c r="E219">
-        <v>0.9789918616978681</v>
+        <v>0.9427968100760467</v>
       </c>
     </row>
     <row r="220" spans="1:5">
@@ -6343,10 +6295,10 @@
         <v>512</v>
       </c>
       <c r="D220">
-        <v>0.9036955522112958</v>
+        <v>0.9459873394555399</v>
       </c>
       <c r="E220">
-        <v>0.9694155953804642</v>
+        <v>0.9740703546282021</v>
       </c>
     </row>
     <row r="221" spans="1:5">
@@ -6360,10 +6312,10 @@
         <v>703</v>
       </c>
       <c r="D221">
-        <v>0.777533211627441</v>
+        <v>0.7782144070837911</v>
       </c>
       <c r="E221">
-        <v>0.9015178181289634</v>
+        <v>0.8930326534096886</v>
       </c>
     </row>
     <row r="222" spans="1:5">
@@ -6377,10 +6329,10 @@
         <v>704</v>
       </c>
       <c r="D222">
-        <v>0.8467676240374041</v>
+        <v>0.792753264853899</v>
       </c>
       <c r="E222">
-        <v>0.9645408273931034</v>
+        <v>0.9307297041720953</v>
       </c>
     </row>
     <row r="223" spans="1:5">
@@ -6394,10 +6346,10 @@
         <v>705</v>
       </c>
       <c r="D223">
-        <v>0.6770990541837034</v>
+        <v>0.5301867850754409</v>
       </c>
       <c r="E223">
-        <v>0.7220938635155941</v>
+        <v>0.4514506747841656</v>
       </c>
     </row>
     <row r="224" spans="1:5">
@@ -6411,10 +6363,10 @@
         <v>706</v>
       </c>
       <c r="D224">
-        <v>0.9022100313930461</v>
+        <v>0.8994826338472753</v>
       </c>
       <c r="E224">
-        <v>0.9492413867887957</v>
+        <v>0.9393340110711592</v>
       </c>
     </row>
     <row r="225" spans="1:5">
@@ -6427,12 +6379,6 @@
       <c r="C225" t="s">
         <v>517</v>
       </c>
-      <c r="D225">
-        <v>0.7438187225882342</v>
-      </c>
-      <c r="E225">
-        <v>0.8065751363923492</v>
-      </c>
     </row>
     <row r="226" spans="1:5">
       <c r="A226" t="s">
@@ -6445,10 +6391,10 @@
         <v>518</v>
       </c>
       <c r="D226">
-        <v>0.9087625056222767</v>
+        <v>0.8700094941337245</v>
       </c>
       <c r="E226">
-        <v>0.8965756184263833</v>
+        <v>0.901620575739921</v>
       </c>
     </row>
     <row r="227" spans="1:5">
@@ -6462,10 +6408,10 @@
         <v>707</v>
       </c>
       <c r="D227">
-        <v>0.6622497672398462</v>
+        <v>0.6912647813481391</v>
       </c>
       <c r="E227">
-        <v>0.7665006383018172</v>
+        <v>0.8724222440308624</v>
       </c>
     </row>
     <row r="228" spans="1:5">
@@ -6479,10 +6425,10 @@
         <v>708</v>
       </c>
       <c r="D228">
-        <v>0.9632375950696768</v>
+        <v>0.9568899386042555</v>
       </c>
       <c r="E228">
-        <v>0.9800030580618897</v>
+        <v>0.9918345289504519</v>
       </c>
     </row>
     <row r="229" spans="1:5">
@@ -6496,10 +6442,10 @@
         <v>521</v>
       </c>
       <c r="D229">
-        <v>0.6894388315046343</v>
+        <v>0.6588142205155151</v>
       </c>
       <c r="E229">
-        <v>0.6283126252873915</v>
+        <v>0.6008068280750911</v>
       </c>
     </row>
     <row r="230" spans="1:5">
@@ -6513,10 +6459,10 @@
         <v>709</v>
       </c>
       <c r="D230">
-        <v>0.6364623546772674</v>
+        <v>0.6950739581247927</v>
       </c>
       <c r="E230">
-        <v>0.6448471320121865</v>
+        <v>0.9272835539599169</v>
       </c>
     </row>
     <row r="231" spans="1:5">
@@ -6530,10 +6476,10 @@
         <v>710</v>
       </c>
       <c r="D231">
-        <v>0.9218911277733218</v>
+        <v>0.9075746320377868</v>
       </c>
       <c r="E231">
-        <v>0.957419269137738</v>
+        <v>0.9493067418627169</v>
       </c>
     </row>
     <row r="232" spans="1:5">
@@ -6547,10 +6493,10 @@
         <v>711</v>
       </c>
       <c r="D232">
-        <v>0.9338278354696601</v>
+        <v>0.9610461046111981</v>
       </c>
       <c r="E232">
-        <v>0.986081512331406</v>
+        <v>0.9681746658047421</v>
       </c>
     </row>
     <row r="233" spans="1:5">
@@ -6564,10 +6510,10 @@
         <v>712</v>
       </c>
       <c r="D233">
-        <v>0.9931173641260723</v>
+        <v>0.9959506081023412</v>
       </c>
       <c r="E233">
-        <v>0.9995319686570603</v>
+        <v>0.9917075886171323</v>
       </c>
     </row>
     <row r="234" spans="1:5">
@@ -6581,10 +6527,10 @@
         <v>713</v>
       </c>
       <c r="D234">
-        <v>0.4205623372841775</v>
+        <v>0.3766839587110271</v>
       </c>
       <c r="E234">
-        <v>0.2989379224257112</v>
+        <v>0.1523359349963496</v>
       </c>
     </row>
     <row r="235" spans="1:5">
@@ -6598,10 +6544,10 @@
         <v>527</v>
       </c>
       <c r="D235">
-        <v>0.5376956970355329</v>
+        <v>0.6397599656478042</v>
       </c>
       <c r="E235">
-        <v>0.7376593991409113</v>
+        <v>0.8961118611417002</v>
       </c>
     </row>
     <row r="236" spans="1:5">
@@ -6615,10 +6561,10 @@
         <v>528</v>
       </c>
       <c r="D236">
-        <v>0.9371038727678836</v>
+        <v>0.9415058341186585</v>
       </c>
       <c r="E236">
-        <v>0.9843521580827171</v>
+        <v>0.9777275587448142</v>
       </c>
     </row>
     <row r="237" spans="1:5">
@@ -6632,10 +6578,10 @@
         <v>714</v>
       </c>
       <c r="D237">
-        <v>0.9495679799100277</v>
+        <v>0.9538593793028061</v>
       </c>
       <c r="E237">
-        <v>0.9620548691706216</v>
+        <v>0.9742990792922257</v>
       </c>
     </row>
     <row r="238" spans="1:5">
@@ -6649,10 +6595,10 @@
         <v>715</v>
       </c>
       <c r="D238">
-        <v>0.973491020665786</v>
+        <v>0.9850038849121151</v>
       </c>
       <c r="E238">
-        <v>0.9988041142652481</v>
+        <v>0.9961314612914443</v>
       </c>
     </row>
     <row r="239" spans="1:5">
@@ -6666,10 +6612,10 @@
         <v>531</v>
       </c>
       <c r="D239">
-        <v>0.6738535824075492</v>
+        <v>0.5923406745669056</v>
       </c>
       <c r="E239">
-        <v>0.5974322205833668</v>
+        <v>0.6862686351566347</v>
       </c>
     </row>
     <row r="240" spans="1:5">
@@ -6683,10 +6629,10 @@
         <v>716</v>
       </c>
       <c r="D240">
-        <v>0.9282531817520895</v>
+        <v>0.9065425284224879</v>
       </c>
       <c r="E240">
-        <v>0.9592300314483813</v>
+        <v>0.9344318344446516</v>
       </c>
     </row>
     <row r="241" spans="1:5">
@@ -6700,10 +6646,10 @@
         <v>533</v>
       </c>
       <c r="D241">
-        <v>0.8326448345549177</v>
+        <v>0.8493485586379139</v>
       </c>
       <c r="E241">
-        <v>0.8041746060311378</v>
+        <v>0.8742183702919242</v>
       </c>
     </row>
     <row r="242" spans="1:5">
@@ -6717,10 +6663,10 @@
         <v>717</v>
       </c>
       <c r="D242">
-        <v>0.2494651375208274</v>
+        <v>0.2481726256886034</v>
       </c>
       <c r="E242">
-        <v>0.1109810278890124</v>
+        <v>0.1442911637948971</v>
       </c>
     </row>
     <row r="243" spans="1:5">
@@ -6734,10 +6680,10 @@
         <v>718</v>
       </c>
       <c r="D243">
-        <v>0.8838445073363516</v>
+        <v>0.907212296347894</v>
       </c>
       <c r="E243">
-        <v>0.9509643923446495</v>
+        <v>0.9621923816680958</v>
       </c>
     </row>
     <row r="244" spans="1:5">
@@ -6751,10 +6697,10 @@
         <v>719</v>
       </c>
       <c r="D244">
-        <v>0.7582749548196397</v>
+        <v>0.7593429659969051</v>
       </c>
       <c r="E244">
-        <v>0.887805252296932</v>
+        <v>0.8715761201497262</v>
       </c>
     </row>
     <row r="245" spans="1:5">
@@ -6768,10 +6714,10 @@
         <v>537</v>
       </c>
       <c r="D245">
-        <v>0.7993729938538364</v>
+        <v>0.7671622110627312</v>
       </c>
       <c r="E245">
-        <v>0.7146951487906703</v>
+        <v>0.7158830889614735</v>
       </c>
     </row>
     <row r="246" spans="1:5">
@@ -6785,10 +6731,10 @@
         <v>538</v>
       </c>
       <c r="D246">
-        <v>0.9506693869262388</v>
+        <v>0.935532708894473</v>
       </c>
       <c r="E246">
-        <v>0.9824289950814036</v>
+        <v>0.9832542917037616</v>
       </c>
     </row>
     <row r="247" spans="1:5">
@@ -6802,10 +6748,10 @@
         <v>539</v>
       </c>
       <c r="D247">
-        <v>0.8422874961192049</v>
+        <v>0.8923625955809411</v>
       </c>
       <c r="E247">
-        <v>0.9600024752348582</v>
+        <v>0.9537838988121828</v>
       </c>
     </row>
     <row r="248" spans="1:5">
@@ -6819,10 +6765,10 @@
         <v>720</v>
       </c>
       <c r="D248">
-        <v>0.8529617526237611</v>
+        <v>0.8420256089513967</v>
       </c>
       <c r="E248">
-        <v>0.9324924598844853</v>
+        <v>0.9439192882847254</v>
       </c>
     </row>
     <row r="249" spans="1:5">
@@ -6836,10 +6782,10 @@
         <v>541</v>
       </c>
       <c r="D249">
-        <v>0.3635850434765417</v>
+        <v>0.3098020629837525</v>
       </c>
       <c r="E249">
-        <v>0.3623082844755015</v>
+        <v>0.09873414337049369</v>
       </c>
     </row>
     <row r="250" spans="1:5">
@@ -6853,10 +6799,10 @@
         <v>542</v>
       </c>
       <c r="D250">
-        <v>0.5120630669939822</v>
+        <v>0.6131781105014964</v>
       </c>
       <c r="E250">
-        <v>0.2409343581482979</v>
+        <v>0.4931355608487083</v>
       </c>
     </row>
     <row r="251" spans="1:5">
@@ -6870,10 +6816,10 @@
         <v>721</v>
       </c>
       <c r="D251">
-        <v>0.8584876632988925</v>
+        <v>0.8548701791809922</v>
       </c>
       <c r="E251">
-        <v>0.9450981196002386</v>
+        <v>0.9066073086524049</v>
       </c>
     </row>
     <row r="252" spans="1:5">
@@ -6887,10 +6833,10 @@
         <v>544</v>
       </c>
       <c r="D252">
-        <v>0.8039924034166098</v>
+        <v>0.8758291863000227</v>
       </c>
       <c r="E252">
-        <v>0.898057128316082</v>
+        <v>0.91250810693634</v>
       </c>
     </row>
     <row r="253" spans="1:5">
@@ -6904,10 +6850,10 @@
         <v>722</v>
       </c>
       <c r="D253">
-        <v>0.1847309983555681</v>
+        <v>0.2316705111835466</v>
       </c>
       <c r="E253">
-        <v>0.490201606511695</v>
+        <v>0.1769711182660007</v>
       </c>
     </row>
     <row r="254" spans="1:5">
@@ -6921,10 +6867,10 @@
         <v>723</v>
       </c>
       <c r="D254">
-        <v>0.8532258156093845</v>
+        <v>0.891449221807099</v>
       </c>
       <c r="E254">
-        <v>0.9288094131605145</v>
+        <v>0.9290850876917036</v>
       </c>
     </row>
     <row r="255" spans="1:5">
@@ -6938,10 +6884,10 @@
         <v>547</v>
       </c>
       <c r="D255">
-        <v>0.8359663295686902</v>
+        <v>0.8739589106408718</v>
       </c>
       <c r="E255">
-        <v>0.8643299430890811</v>
+        <v>0.9357809064594291</v>
       </c>
     </row>
     <row r="256" spans="1:5">
@@ -6955,10 +6901,10 @@
         <v>724</v>
       </c>
       <c r="D256">
-        <v>0.8760986753277428</v>
+        <v>0.8464988736220271</v>
       </c>
       <c r="E256">
-        <v>0.8030132261344847</v>
+        <v>0.927931211593504</v>
       </c>
     </row>
     <row r="257" spans="1:5">
@@ -6972,10 +6918,10 @@
         <v>725</v>
       </c>
       <c r="D257">
-        <v>0.8627910488766251</v>
+        <v>0.9395542784168995</v>
       </c>
       <c r="E257">
-        <v>0.9038610402040806</v>
+        <v>0.9495515252386263</v>
       </c>
     </row>
     <row r="258" spans="1:5">
@@ -6989,10 +6935,10 @@
         <v>550</v>
       </c>
       <c r="D258">
-        <v>0.7555034458972506</v>
+        <v>0.8737906175511398</v>
       </c>
       <c r="E258">
-        <v>0.8874632899153103</v>
+        <v>0.9483854960980066</v>
       </c>
     </row>
     <row r="259" spans="1:5">
@@ -7006,10 +6952,10 @@
         <v>726</v>
       </c>
       <c r="D259">
-        <v>0.8098693102905169</v>
+        <v>0.7979789855870014</v>
       </c>
       <c r="E259">
-        <v>0.840059722474513</v>
+        <v>0.7960321248405359</v>
       </c>
     </row>
     <row r="260" spans="1:5">
@@ -7023,10 +6969,10 @@
         <v>552</v>
       </c>
       <c r="D260">
-        <v>0.7921457844506989</v>
+        <v>0.6864211961591622</v>
       </c>
       <c r="E260">
-        <v>0.6075309848477073</v>
+        <v>0.5912035685487287</v>
       </c>
     </row>
     <row r="261" spans="1:5">
@@ -7040,10 +6986,10 @@
         <v>727</v>
       </c>
       <c r="D261">
-        <v>0.7084667999056606</v>
+        <v>0.7955950774351477</v>
       </c>
       <c r="E261">
-        <v>0.9092204930140014</v>
+        <v>0.9096285678189183</v>
       </c>
     </row>
     <row r="262" spans="1:5">
@@ -7057,10 +7003,10 @@
         <v>728</v>
       </c>
       <c r="D262">
-        <v>0.7651453731021723</v>
+        <v>0.8575543129239864</v>
       </c>
       <c r="E262">
-        <v>0.8837817189118033</v>
+        <v>0.9345469471300255</v>
       </c>
     </row>
     <row r="263" spans="1:5">
@@ -7074,10 +7020,10 @@
         <v>729</v>
       </c>
       <c r="D263">
-        <v>0.9629182640517093</v>
+        <v>0.9748131133669217</v>
       </c>
       <c r="E263">
-        <v>0.9815648869329556</v>
+        <v>0.989412099572209</v>
       </c>
     </row>
     <row r="264" spans="1:5">
@@ -7091,10 +7037,10 @@
         <v>556</v>
       </c>
       <c r="D264">
-        <v>0.9632415809742504</v>
+        <v>0.9137101074610101</v>
       </c>
       <c r="E264">
-        <v>0.9823746784517856</v>
+        <v>0.9250388581391188</v>
       </c>
     </row>
     <row r="265" spans="1:5">
@@ -7108,10 +7054,10 @@
         <v>730</v>
       </c>
       <c r="D265">
-        <v>0.6072002875875436</v>
+        <v>0.4450174477301443</v>
       </c>
       <c r="E265">
-        <v>0.8058702510186797</v>
+        <v>0.6189535676339867</v>
       </c>
     </row>
     <row r="266" spans="1:5">
@@ -7125,10 +7071,10 @@
         <v>731</v>
       </c>
       <c r="D266">
-        <v>0.9227221696367751</v>
+        <v>0.9410819890331272</v>
       </c>
       <c r="E266">
-        <v>0.9601984492539825</v>
+        <v>0.9838662827551354</v>
       </c>
     </row>
     <row r="267" spans="1:5">
@@ -7142,10 +7088,10 @@
         <v>732</v>
       </c>
       <c r="D267">
-        <v>0.8343735355374683</v>
+        <v>0.7952623887288829</v>
       </c>
       <c r="E267">
-        <v>0.8986038150050856</v>
+        <v>0.9155074409169871</v>
       </c>
     </row>
     <row r="268" spans="1:5">
@@ -7159,10 +7105,10 @@
         <v>733</v>
       </c>
       <c r="D268">
-        <v>0.6638936192740643</v>
+        <v>0.6076224531661916</v>
       </c>
       <c r="E268">
-        <v>0.5642182503935307</v>
+        <v>0.5493812330942554</v>
       </c>
     </row>
     <row r="269" spans="1:5">
@@ -7176,10 +7122,10 @@
         <v>561</v>
       </c>
       <c r="D269">
-        <v>0.6474127344581684</v>
+        <v>0.754572489795177</v>
       </c>
       <c r="E269">
-        <v>0.8201780959265024</v>
+        <v>0.8276053096459497</v>
       </c>
     </row>
     <row r="270" spans="1:5">
@@ -7193,10 +7139,10 @@
         <v>562</v>
       </c>
       <c r="D270">
-        <v>0.9717450361851628</v>
+        <v>0.9482289167328904</v>
       </c>
       <c r="E270">
-        <v>0.9954755450834913</v>
+        <v>0.9857988983814338</v>
       </c>
     </row>
     <row r="271" spans="1:5">
@@ -7210,10 +7156,10 @@
         <v>734</v>
       </c>
       <c r="D271">
-        <v>0.287046229507427</v>
+        <v>0.3109001445169268</v>
       </c>
       <c r="E271">
-        <v>0.217795350170065</v>
+        <v>0.1484305882875757</v>
       </c>
     </row>
     <row r="272" spans="1:5">
@@ -7227,10 +7173,10 @@
         <v>735</v>
       </c>
       <c r="D272">
-        <v>0.8088272611532865</v>
+        <v>0.7878511742087738</v>
       </c>
       <c r="E272">
-        <v>0.6949697582456392</v>
+        <v>0.7553960432409271</v>
       </c>
     </row>
     <row r="273" spans="1:5">
@@ -7244,10 +7190,10 @@
         <v>736</v>
       </c>
       <c r="D273">
-        <v>0.7625957854005501</v>
+        <v>0.7617923337306166</v>
       </c>
       <c r="E273">
-        <v>0.8478555338438325</v>
+        <v>0.8659660514730682</v>
       </c>
     </row>
     <row r="274" spans="1:5">
@@ -7261,10 +7207,10 @@
         <v>566</v>
       </c>
       <c r="D274">
-        <v>0.5871313693934391</v>
+        <v>0.5591362763228412</v>
       </c>
       <c r="E274">
-        <v>0.6667011511328653</v>
+        <v>0.7092674705710444</v>
       </c>
     </row>
     <row r="275" spans="1:5">
@@ -7278,10 +7224,10 @@
         <v>737</v>
       </c>
       <c r="D275">
-        <v>0.6208491015613109</v>
+        <v>0.4861201759661735</v>
       </c>
       <c r="E275">
-        <v>0.6706887544563138</v>
+        <v>0.6687135324863663</v>
       </c>
     </row>
     <row r="276" spans="1:5">
@@ -7295,10 +7241,10 @@
         <v>738</v>
       </c>
       <c r="D276">
-        <v>0.8306282091567928</v>
+        <v>0.8172739072383453</v>
       </c>
       <c r="E276">
-        <v>0.8834300477505805</v>
+        <v>0.9073838894374711</v>
       </c>
     </row>
     <row r="277" spans="1:5">
@@ -7312,10 +7258,10 @@
         <v>739</v>
       </c>
       <c r="D277">
-        <v>0.818190721770767</v>
+        <v>0.6772332852083652</v>
       </c>
       <c r="E277">
-        <v>0.9222183926067166</v>
+        <v>0.721926439803404</v>
       </c>
     </row>
     <row r="278" spans="1:5">
@@ -7329,10 +7275,10 @@
         <v>570</v>
       </c>
       <c r="D278">
-        <v>0.8437664151671235</v>
+        <v>0.8594064700315769</v>
       </c>
       <c r="E278">
-        <v>0.940047733877858</v>
+        <v>0.9424185131011342</v>
       </c>
     </row>
     <row r="279" spans="1:5">
@@ -7346,10 +7292,10 @@
         <v>571</v>
       </c>
       <c r="D279">
-        <v>0.7239480493929543</v>
+        <v>0.7511934824104556</v>
       </c>
       <c r="E279">
-        <v>0.8191566659714299</v>
+        <v>0.8160691901313375</v>
       </c>
     </row>
     <row r="280" spans="1:5">
@@ -7363,10 +7309,10 @@
         <v>572</v>
       </c>
       <c r="D280">
-        <v>0.4158232063583875</v>
+        <v>0.3100351703608648</v>
       </c>
       <c r="E280">
-        <v>0.1447011311162399</v>
+        <v>0.1406559823015656</v>
       </c>
     </row>
     <row r="281" spans="1:5">
@@ -7380,10 +7326,10 @@
         <v>740</v>
       </c>
       <c r="D281">
-        <v>0.7726505864361792</v>
+        <v>0.6793329138557234</v>
       </c>
       <c r="E281">
-        <v>0.8362767038823808</v>
+        <v>0.8264803464648406</v>
       </c>
     </row>
     <row r="282" spans="1:5">
@@ -7397,10 +7343,10 @@
         <v>741</v>
       </c>
       <c r="D282">
-        <v>0.8799888556975156</v>
+        <v>0.9284737731840189</v>
       </c>
       <c r="E282">
-        <v>0.9271224534515972</v>
+        <v>0.9773851009300957</v>
       </c>
     </row>
     <row r="283" spans="1:5">
@@ -7414,10 +7360,10 @@
         <v>575</v>
       </c>
       <c r="D283">
-        <v>0.6599408700947129</v>
+        <v>0.6925234248061982</v>
       </c>
       <c r="E283">
-        <v>0.7884390263998663</v>
+        <v>0.8627196681119402</v>
       </c>
     </row>
     <row r="284" spans="1:5">
@@ -7431,10 +7377,10 @@
         <v>576</v>
       </c>
       <c r="D284">
-        <v>0.6846166068617991</v>
+        <v>0.6652933719954395</v>
       </c>
       <c r="E284">
-        <v>0.8464491032570565</v>
+        <v>0.7909630270092267</v>
       </c>
     </row>
     <row r="285" spans="1:5">
@@ -7448,10 +7394,10 @@
         <v>742</v>
       </c>
       <c r="D285">
-        <v>0.9366785681131217</v>
+        <v>0.9308741444569072</v>
       </c>
       <c r="E285">
-        <v>0.9873216460162265</v>
+        <v>0.9728328945852912</v>
       </c>
     </row>
     <row r="286" spans="1:5">
@@ -7465,10 +7411,10 @@
         <v>578</v>
       </c>
       <c r="D286">
-        <v>0.4007909818038048</v>
+        <v>0.259043080198628</v>
       </c>
       <c r="E286">
-        <v>0.1550026712250019</v>
+        <v>0.1707525564529866</v>
       </c>
     </row>
     <row r="287" spans="1:5">
@@ -7482,10 +7428,10 @@
         <v>743</v>
       </c>
       <c r="D287">
-        <v>0.715333214132274</v>
+        <v>0.7620976523582926</v>
       </c>
       <c r="E287">
-        <v>0.6621446385768155</v>
+        <v>0.8366500731997031</v>
       </c>
     </row>
     <row r="288" spans="1:5">
@@ -7498,12 +7444,6 @@
       <c r="C288" t="s">
         <v>580</v>
       </c>
-      <c r="D288">
-        <v>0.6118854012536451</v>
-      </c>
-      <c r="E288">
-        <v>0.4995299317866036</v>
-      </c>
     </row>
     <row r="289" spans="1:5">
       <c r="A289" t="s">
@@ -7516,10 +7456,10 @@
         <v>744</v>
       </c>
       <c r="D289">
-        <v>0.9342106301189614</v>
+        <v>0.9324513551036916</v>
       </c>
       <c r="E289">
-        <v>0.8887650212953772</v>
+        <v>0.9651421698372669</v>
       </c>
     </row>
     <row r="290" spans="1:5">
@@ -7533,10 +7473,10 @@
         <v>745</v>
       </c>
       <c r="D290">
-        <v>0.6272600627949332</v>
+        <v>0.896697291908343</v>
       </c>
       <c r="E290">
-        <v>0.4768598610259543</v>
+        <v>0.8939650345917928</v>
       </c>
     </row>
     <row r="291" spans="1:5">
@@ -7550,10 +7490,10 @@
         <v>746</v>
       </c>
       <c r="D291">
-        <v>0.8479685184230051</v>
+        <v>0.9301201595687696</v>
       </c>
       <c r="E291">
-        <v>0.9213555149785172</v>
+        <v>0.9664117073835023</v>
       </c>
     </row>
   </sheetData>

</xml_diff>